<commit_message>
noelia ha cambiado de user en codewars
</commit_message>
<xml_diff>
--- a/output/output.xlsx
+++ b/output/output.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
   <si>
     <t>sql-with-sailor-moon-thinking-about-joins-dot-dot-dot</t>
   </si>
@@ -22,6 +22,9 @@
     <t>80-s-kids-number-2-help-alf-find-his-spaceship</t>
   </si>
   <si>
+    <t>filter-out-the-geese</t>
+  </si>
+  <si>
     <t>username</t>
   </si>
   <si>
@@ -58,7 +61,7 @@
     <t>CMFV</t>
   </si>
   <si>
-    <t>noeliacarrion</t>
+    <t>nihal.99</t>
   </si>
   <si>
     <t>Leticiazcu</t>
@@ -440,26 +443,29 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C21"/>
+  <dimension ref="A1:D21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:4">
       <c r="A1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3">
+    </row>
+    <row r="2" spans="1:4">
       <c r="A2" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B2" t="b">
         <v>1</v>
@@ -467,10 +473,13 @@
       <c r="C2" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:3">
+      <c r="D2" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
       <c r="A3" s="1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B3" t="b">
         <v>1</v>
@@ -478,10 +487,13 @@
       <c r="C3" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:3">
+      <c r="D3" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
       <c r="A4" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B4" t="b">
         <v>1</v>
@@ -489,10 +501,13 @@
       <c r="C4" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:3">
+      <c r="D4" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
       <c r="A5" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B5" t="b">
         <v>1</v>
@@ -500,10 +515,13 @@
       <c r="C5" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="6" spans="1:3">
+      <c r="D5" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
       <c r="A6" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B6" t="b">
         <v>1</v>
@@ -511,10 +529,13 @@
       <c r="C6" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="7" spans="1:3">
+      <c r="D6" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
       <c r="A7" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B7" t="b">
         <v>1</v>
@@ -522,10 +543,13 @@
       <c r="C7" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="8" spans="1:3">
+      <c r="D7" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
       <c r="A8" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B8" t="b">
         <v>1</v>
@@ -533,10 +557,13 @@
       <c r="C8" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="9" spans="1:3">
+      <c r="D8" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
       <c r="A9" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B9" t="b">
         <v>1</v>
@@ -544,10 +571,13 @@
       <c r="C9" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="10" spans="1:3">
+      <c r="D9" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
       <c r="A10" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B10" t="b">
         <v>0</v>
@@ -555,10 +585,13 @@
       <c r="C10" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="11" spans="1:3">
+      <c r="D10" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4">
       <c r="A11" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B11" t="b">
         <v>1</v>
@@ -566,10 +599,13 @@
       <c r="C11" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="12" spans="1:3">
+      <c r="D11" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4">
       <c r="A12" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B12" t="b">
         <v>1</v>
@@ -577,10 +613,13 @@
       <c r="C12" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="13" spans="1:3">
+      <c r="D12" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4">
       <c r="A13" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B13" t="b">
         <v>1</v>
@@ -588,10 +627,13 @@
       <c r="C13" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="14" spans="1:3">
+      <c r="D13" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4">
       <c r="A14" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B14" t="b">
         <v>1</v>
@@ -599,10 +641,13 @@
       <c r="C14" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="15" spans="1:3">
+      <c r="D14" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4">
       <c r="A15" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B15" t="b">
         <v>1</v>
@@ -610,10 +655,13 @@
       <c r="C15" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="16" spans="1:3">
+      <c r="D15" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4">
       <c r="A16" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B16" t="b">
         <v>1</v>
@@ -621,10 +669,13 @@
       <c r="C16" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="17" spans="1:3">
+      <c r="D16" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4">
       <c r="A17" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B17" t="b">
         <v>1</v>
@@ -632,10 +683,13 @@
       <c r="C17" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="18" spans="1:3">
+      <c r="D17" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4">
       <c r="A18" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B18" t="b">
         <v>1</v>
@@ -643,10 +697,13 @@
       <c r="C18" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="19" spans="1:3">
+      <c r="D18" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4">
       <c r="A19" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B19" t="b">
         <v>1</v>
@@ -654,10 +711,13 @@
       <c r="C19" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="20" spans="1:3">
+      <c r="D19" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4">
       <c r="A20" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B20" t="b">
         <v>1</v>
@@ -665,16 +725,22 @@
       <c r="C20" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="21" spans="1:3">
+      <c r="D20" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4">
       <c r="A21" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B21" t="b">
         <v>1</v>
       </c>
       <c r="C21" t="b">
         <v>0</v>
+      </c>
+      <c r="D21" t="b">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
ahora el CSV puede tener espacios
</commit_message>
<xml_diff>
--- a/output/output.xlsx
+++ b/output/output.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
   <si>
     <t>sql-with-sailor-moon-thinking-about-joins-dot-dot-dot</t>
   </si>
@@ -26,6 +26,9 @@
   </si>
   <si>
     <t>sql-basics-monsters-using-case</t>
+  </si>
+  <si>
+    <t>alphabet-war</t>
   </si>
   <si>
     <t>username</t>
@@ -446,15 +449,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E21"/>
+  <dimension ref="A1:F21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:6">
       <c r="A1" s="1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -468,10 +471,13 @@
       <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:5">
+      <c r="F1" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
       <c r="A2" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B2" t="b">
         <v>1</v>
@@ -485,10 +491,13 @@
       <c r="E2" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:5">
+      <c r="F2" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
       <c r="A3" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B3" t="b">
         <v>1</v>
@@ -502,10 +511,13 @@
       <c r="E3" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:5">
+      <c r="F3" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
       <c r="A4" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B4" t="b">
         <v>1</v>
@@ -517,12 +529,15 @@
         <v>1</v>
       </c>
       <c r="E4" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5">
+        <v>1</v>
+      </c>
+      <c r="F4" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
       <c r="A5" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B5" t="b">
         <v>1</v>
@@ -536,10 +551,13 @@
       <c r="E5" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="6" spans="1:5">
+      <c r="F5" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
       <c r="A6" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B6" t="b">
         <v>1</v>
@@ -551,12 +569,15 @@
         <v>1</v>
       </c>
       <c r="E6" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5">
+        <v>1</v>
+      </c>
+      <c r="F6" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
       <c r="A7" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B7" t="b">
         <v>1</v>
@@ -570,10 +591,13 @@
       <c r="E7" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="8" spans="1:5">
+      <c r="F7" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
       <c r="A8" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B8" t="b">
         <v>1</v>
@@ -585,12 +609,15 @@
         <v>1</v>
       </c>
       <c r="E8" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5">
+        <v>1</v>
+      </c>
+      <c r="F8" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
       <c r="A9" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B9" t="b">
         <v>1</v>
@@ -602,12 +629,15 @@
         <v>1</v>
       </c>
       <c r="E9" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5">
+        <v>1</v>
+      </c>
+      <c r="F9" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
       <c r="A10" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B10" t="b">
         <v>0</v>
@@ -621,10 +651,13 @@
       <c r="E10" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="11" spans="1:5">
+      <c r="F10" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6">
       <c r="A11" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B11" t="b">
         <v>1</v>
@@ -638,10 +671,13 @@
       <c r="E11" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="12" spans="1:5">
+      <c r="F11" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6">
       <c r="A12" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B12" t="b">
         <v>1</v>
@@ -653,12 +689,15 @@
         <v>1</v>
       </c>
       <c r="E12" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5">
+        <v>1</v>
+      </c>
+      <c r="F12" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6">
       <c r="A13" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B13" t="b">
         <v>1</v>
@@ -670,12 +709,15 @@
         <v>1</v>
       </c>
       <c r="E13" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5">
+        <v>1</v>
+      </c>
+      <c r="F13" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6">
       <c r="A14" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B14" t="b">
         <v>1</v>
@@ -689,10 +731,13 @@
       <c r="E14" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="15" spans="1:5">
+      <c r="F14" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6">
       <c r="A15" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B15" t="b">
         <v>1</v>
@@ -704,12 +749,15 @@
         <v>1</v>
       </c>
       <c r="E15" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5">
+        <v>1</v>
+      </c>
+      <c r="F15" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6">
       <c r="A16" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B16" t="b">
         <v>1</v>
@@ -721,12 +769,15 @@
         <v>1</v>
       </c>
       <c r="E16" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5">
+        <v>1</v>
+      </c>
+      <c r="F16" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6">
       <c r="A17" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B17" t="b">
         <v>1</v>
@@ -740,10 +791,13 @@
       <c r="E17" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="18" spans="1:5">
+      <c r="F17" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6">
       <c r="A18" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B18" t="b">
         <v>1</v>
@@ -755,12 +809,15 @@
         <v>1</v>
       </c>
       <c r="E18" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5">
+        <v>1</v>
+      </c>
+      <c r="F18" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6">
       <c r="A19" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B19" t="b">
         <v>1</v>
@@ -772,12 +829,15 @@
         <v>1</v>
       </c>
       <c r="E19" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5">
+        <v>1</v>
+      </c>
+      <c r="F19" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6">
       <c r="A20" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B20" t="b">
         <v>1</v>
@@ -789,12 +849,15 @@
         <v>1</v>
       </c>
       <c r="E20" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5">
+        <v>1</v>
+      </c>
+      <c r="F20" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6">
       <c r="A21" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B21" t="b">
         <v>1</v>
@@ -806,6 +869,9 @@
         <v>1</v>
       </c>
       <c r="E21" t="b">
+        <v>1</v>
+      </c>
+      <c r="F21" t="b">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Kata 2-3, Modificacion excel good/no
</commit_message>
<xml_diff>
--- a/output/output.xlsx
+++ b/output/output.xlsx
@@ -358,7 +358,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C29"/>
+  <dimension ref="A1:D29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -379,7 +379,12 @@
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>tests-results</t>
+          <t>sum-mixed-array</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>keep-hydrated-1</t>
         </is>
       </c>
     </row>
@@ -389,11 +394,20 @@
           <t>Maika7</t>
         </is>
       </c>
-      <c r="B2" t="b">
-        <v>0</v>
-      </c>
-      <c r="C2" t="b">
-        <v>0</v>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>Good</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>Good</t>
+        </is>
       </c>
     </row>
     <row r="3">
@@ -402,11 +416,20 @@
           <t>Ovión</t>
         </is>
       </c>
-      <c r="B3" t="b">
-        <v>1</v>
-      </c>
-      <c r="C3" t="b">
-        <v>0</v>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>Good</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>Good</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>Good</t>
+        </is>
       </c>
     </row>
     <row r="4">
@@ -415,11 +438,20 @@
           <t>mariadrados</t>
         </is>
       </c>
-      <c r="B4" t="b">
-        <v>1</v>
-      </c>
-      <c r="C4" t="b">
-        <v>0</v>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Good</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>Good</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>Good</t>
+        </is>
       </c>
     </row>
     <row r="5">
@@ -428,11 +460,20 @@
           <t>jlmingo</t>
         </is>
       </c>
-      <c r="B5" t="b">
-        <v>1</v>
-      </c>
-      <c r="C5" t="b">
-        <v>0</v>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>Good</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>Good</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>Good</t>
+        </is>
       </c>
     </row>
     <row r="6">
@@ -441,11 +482,20 @@
           <t>seorakwon</t>
         </is>
       </c>
-      <c r="B6" t="b">
-        <v>1</v>
-      </c>
-      <c r="C6" t="b">
-        <v>0</v>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>Good</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
       </c>
     </row>
     <row r="7">
@@ -454,11 +504,20 @@
           <t>ladyCelia</t>
         </is>
       </c>
-      <c r="B7" t="b">
-        <v>1</v>
-      </c>
-      <c r="C7" t="b">
-        <v>0</v>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>Good</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>Good</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>Good</t>
+        </is>
       </c>
     </row>
     <row r="8">
@@ -467,11 +526,20 @@
           <t>castares</t>
         </is>
       </c>
-      <c r="B8" t="b">
-        <v>1</v>
-      </c>
-      <c r="C8" t="b">
-        <v>0</v>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
       </c>
     </row>
     <row r="9">
@@ -480,11 +548,20 @@
           <t>jgph91</t>
         </is>
       </c>
-      <c r="B9" t="b">
-        <v>1</v>
-      </c>
-      <c r="C9" t="b">
-        <v>0</v>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>Good</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>Good</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>Good</t>
+        </is>
       </c>
     </row>
     <row r="10">
@@ -493,11 +570,20 @@
           <t>Clapiniella</t>
         </is>
       </c>
-      <c r="B10" t="b">
-        <v>0</v>
-      </c>
-      <c r="C10" t="b">
-        <v>0</v>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>Good</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
       </c>
     </row>
     <row r="11">
@@ -506,11 +592,20 @@
           <t>AlexMendez13</t>
         </is>
       </c>
-      <c r="B11" t="b">
-        <v>1</v>
-      </c>
-      <c r="C11" t="b">
-        <v>0</v>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>Good</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>Good</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>Good</t>
+        </is>
       </c>
     </row>
     <row r="12">
@@ -519,11 +614,20 @@
           <t>blancaalcala</t>
         </is>
       </c>
-      <c r="B12" t="b">
-        <v>1</v>
-      </c>
-      <c r="C12" t="b">
-        <v>0</v>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>Good</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>Good</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>Good</t>
+        </is>
       </c>
     </row>
     <row r="13">
@@ -532,11 +636,20 @@
           <t>juliopdata</t>
         </is>
       </c>
-      <c r="B13" t="b">
-        <v>1</v>
-      </c>
-      <c r="C13" t="b">
-        <v>0</v>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>Good</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>Good</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>Good</t>
+        </is>
       </c>
     </row>
     <row r="14">
@@ -545,11 +658,20 @@
           <t>alfpml</t>
         </is>
       </c>
-      <c r="B14" t="b">
-        <v>1</v>
-      </c>
-      <c r="C14" t="b">
-        <v>0</v>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
       </c>
     </row>
     <row r="15">
@@ -558,11 +680,20 @@
           <t>Salazar29</t>
         </is>
       </c>
-      <c r="B15" t="b">
-        <v>1</v>
-      </c>
-      <c r="C15" t="b">
-        <v>0</v>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>Good</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>Good</t>
+        </is>
       </c>
     </row>
     <row r="16">
@@ -571,11 +702,20 @@
           <t>mariobru</t>
         </is>
       </c>
-      <c r="B16" t="b">
-        <v>1</v>
-      </c>
-      <c r="C16" t="b">
-        <v>0</v>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>Good</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>Good</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>Good</t>
+        </is>
       </c>
     </row>
     <row r="17">
@@ -584,11 +724,20 @@
           <t>alvarorivasg</t>
         </is>
       </c>
-      <c r="B17" t="b">
-        <v>1</v>
-      </c>
-      <c r="C17" t="b">
-        <v>0</v>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>Good</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>Good</t>
+        </is>
       </c>
     </row>
     <row r="18">
@@ -597,11 +746,20 @@
           <t>jmcruz</t>
         </is>
       </c>
-      <c r="B18" t="b">
-        <v>0</v>
-      </c>
-      <c r="C18" t="b">
-        <v>0</v>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>Good</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
       </c>
     </row>
     <row r="19">
@@ -610,11 +768,20 @@
           <t>guzmanueco</t>
         </is>
       </c>
-      <c r="B19" t="b">
-        <v>1</v>
-      </c>
-      <c r="C19" t="b">
-        <v>0</v>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>Good</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>Good</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>Good</t>
+        </is>
       </c>
     </row>
     <row r="20">
@@ -623,11 +790,20 @@
           <t>DavFer</t>
         </is>
       </c>
-      <c r="B20" t="b">
-        <v>0</v>
-      </c>
-      <c r="C20" t="b">
-        <v>0</v>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>Good</t>
+        </is>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
       </c>
     </row>
     <row r="21">
@@ -636,11 +812,20 @@
           <t>toninopons</t>
         </is>
       </c>
-      <c r="B21" t="b">
-        <v>0</v>
-      </c>
-      <c r="C21" t="b">
-        <v>0</v>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>Good</t>
+        </is>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>Good</t>
+        </is>
       </c>
     </row>
     <row r="22">
@@ -649,11 +834,20 @@
           <t>mmora-fi</t>
         </is>
       </c>
-      <c r="B22" t="b">
-        <v>1</v>
-      </c>
-      <c r="C22" t="b">
-        <v>0</v>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>Good</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>Good</t>
+        </is>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>Good</t>
+        </is>
       </c>
     </row>
     <row r="23">
@@ -662,11 +856,20 @@
           <t>Masdevallia</t>
         </is>
       </c>
-      <c r="B23" t="b">
-        <v>1</v>
-      </c>
-      <c r="C23" t="b">
-        <v>0</v>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>Good</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>Good</t>
+        </is>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>Good</t>
+        </is>
       </c>
     </row>
     <row r="24">
@@ -675,11 +878,20 @@
           <t>Programeitor</t>
         </is>
       </c>
-      <c r="B24" t="b">
-        <v>0</v>
-      </c>
-      <c r="C24" t="b">
-        <v>0</v>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>Good</t>
+        </is>
+      </c>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>Good</t>
+        </is>
       </c>
     </row>
     <row r="25">
@@ -688,11 +900,20 @@
           <t>Mohusty</t>
         </is>
       </c>
-      <c r="B25" t="b">
-        <v>1</v>
-      </c>
-      <c r="C25" t="b">
-        <v>0</v>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>Good</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>Good</t>
+        </is>
+      </c>
+      <c r="D25" t="inlineStr">
+        <is>
+          <t>Good</t>
+        </is>
       </c>
     </row>
     <row r="26">
@@ -701,11 +922,20 @@
           <t>vforvargas</t>
         </is>
       </c>
-      <c r="B26" t="b">
-        <v>0</v>
-      </c>
-      <c r="C26" t="b">
-        <v>0</v>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>Good</t>
+        </is>
+      </c>
+      <c r="D26" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
       </c>
     </row>
     <row r="27">
@@ -714,11 +944,20 @@
           <t>blancalluch</t>
         </is>
       </c>
-      <c r="B27" t="b">
-        <v>0</v>
-      </c>
-      <c r="C27" t="b">
-        <v>0</v>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>Good</t>
+        </is>
+      </c>
+      <c r="D27" t="inlineStr">
+        <is>
+          <t>Good</t>
+        </is>
       </c>
     </row>
     <row r="28">
@@ -727,11 +966,20 @@
           <t>isagc</t>
         </is>
       </c>
-      <c r="B28" t="b">
-        <v>1</v>
-      </c>
-      <c r="C28" t="b">
-        <v>0</v>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>Good</t>
+        </is>
+      </c>
+      <c r="D28" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
       </c>
     </row>
     <row r="29">
@@ -740,11 +988,20 @@
           <t>mariaversin</t>
         </is>
       </c>
-      <c r="B29" t="b">
-        <v>0</v>
-      </c>
-      <c r="C29" t="b">
-        <v>0</v>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>Good</t>
+        </is>
+      </c>
+      <c r="D29" t="inlineStr">
+        <is>
+          <t>Good</t>
+        </is>
       </c>
     </row>
   </sheetData>

</xml_diff>